<commit_message>
edit the sheet name test
</commit_message>
<xml_diff>
--- a/data/dates/Document_Filing_Dates.xlsx
+++ b/data/dates/Document_Filing_Dates.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayu\Desktop\Projects\ay_OilGasEarnings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Documents\Data_Analytics\OilGasEarningsAnalysis\data\dates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62A99CC-1FB8-44AF-9370-91E1D815E9A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F0CE43-DA0B-40D8-977E-6A7FEFACC4B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="862" xr2:uid="{3EA98B58-5733-425D-AE44-6276CE9C3BA9}"/>
+    <workbookView xWindow="368" yWindow="968" windowWidth="10260" windowHeight="8460" tabRatio="862" activeTab="3" xr2:uid="{3EA98B58-5733-425D-AE44-6276CE9C3BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="15" r:id="rId1"/>
     <sheet name="FANG" sheetId="1" r:id="rId2"/>
-    <sheet name="RSPP see note" sheetId="2" r:id="rId3"/>
+    <sheet name="RSPP" sheetId="2" r:id="rId3"/>
     <sheet name="CXO see note" sheetId="3" r:id="rId4"/>
     <sheet name="CEO see note" sheetId="4" r:id="rId5"/>
     <sheet name="MDU" sheetId="5" r:id="rId6"/>
@@ -41,7 +41,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'NFX see note'!$A$3:$B$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PE!$A$1:$B$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">RRC!$A$1:$B$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RSPP see note'!$A$1:$B$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RSPP!$A$1:$B$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'SM (added for me if possible)'!$A$1:$B$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,8 +180,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{DEDE5034-341B-4FD6-A6DB-92EACE4D8559}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -492,48 +520,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4347CB-D72A-415A-B9FD-4EDC7C72C60F}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="O6" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="O7" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="O8" s="4" t="s">
         <v>19</v>
       </c>
@@ -551,12 +579,12 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -564,7 +592,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -572,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -580,7 +608,7 @@
         <v>41698</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -588,7 +616,7 @@
         <v>41759</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -596,7 +624,7 @@
         <v>41850</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -604,7 +632,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -612,7 +640,7 @@
         <v>42059</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -620,7 +648,7 @@
         <v>42130</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -628,7 +656,7 @@
         <v>42221</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -636,7 +664,7 @@
         <v>42312</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -644,7 +672,7 @@
         <v>42424</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -652,7 +680,7 @@
         <v>42493</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -660,7 +688,7 @@
         <v>42585</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -668,7 +696,7 @@
         <v>42675</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -676,7 +704,7 @@
         <v>42787</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -684,7 +712,7 @@
         <v>42857</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -692,7 +720,7 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -700,7 +728,7 @@
         <v>43039</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -708,7 +736,7 @@
         <v>43151</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -716,7 +744,7 @@
         <v>43221</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -724,7 +752,7 @@
         <v>43312</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -753,22 +781,22 @@
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="E2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -776,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -784,7 +812,7 @@
         <v>42793</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -792,7 +820,7 @@
         <v>42859</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -800,7 +828,7 @@
         <v>42941</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -808,7 +836,7 @@
         <v>43048</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -816,7 +844,7 @@
         <v>43157</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -824,7 +852,7 @@
         <v>43223</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -832,7 +860,7 @@
         <v>43314</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -840,7 +868,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -848,7 +876,7 @@
         <v>43524</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -856,31 +884,31 @@
         <v>43587</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B22" s="3"/>
     </row>
   </sheetData>
@@ -901,12 +929,12 @@
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -914,7 +942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -922,7 +950,7 @@
         <v>41698</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -930,7 +958,7 @@
         <v>41768</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -938,7 +966,7 @@
         <v>41858</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -946,7 +974,7 @@
         <v>41950</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -954,7 +982,7 @@
         <v>42062</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -962,7 +990,7 @@
         <v>42131</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -970,7 +998,7 @@
         <v>42223</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -978,7 +1006,7 @@
         <v>42313</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -986,7 +1014,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -994,7 +1022,7 @@
         <v>42495</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1002,7 +1030,7 @@
         <v>42587</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1010,7 +1038,7 @@
         <v>42677</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1046,7 @@
         <v>42781</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1026,7 +1054,7 @@
         <v>42864</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1034,7 +1062,7 @@
         <v>42956</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1042,7 +1070,7 @@
         <v>43041</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1050,7 +1078,7 @@
         <v>43153</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1058,7 +1086,7 @@
         <v>43229</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1066,7 +1094,7 @@
         <v>43314</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1074,7 +1102,7 @@
         <v>43405</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1082,7 +1110,7 @@
         <v>43524</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1108,12 +1136,12 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1121,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1129,7 +1157,7 @@
         <v>41696</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1137,7 +1165,7 @@
         <v>41757</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1145,7 +1173,7 @@
         <v>41813</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1153,7 +1181,7 @@
         <v>41848</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1161,7 +1189,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1169,7 +1197,7 @@
         <v>42059</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1177,7 +1205,7 @@
         <v>42122</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1185,7 +1213,7 @@
         <v>42213</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1193,7 +1221,7 @@
         <v>42305</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1201,7 +1229,7 @@
         <v>42425</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1209,7 +1237,7 @@
         <v>42488</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1217,7 +1245,7 @@
         <v>42577</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1225,7 +1253,7 @@
         <v>42668</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1233,7 +1261,7 @@
         <v>42690</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1241,7 +1269,7 @@
         <v>42788</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1249,7 +1277,7 @@
         <v>42849</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1257,7 +1285,7 @@
         <v>42948</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1265,7 +1293,7 @@
         <v>43032</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1301,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1281,7 +1309,7 @@
         <v>43215</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1289,7 +1317,7 @@
         <v>43311</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1297,7 +1325,7 @@
         <v>43396</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1305,7 +1333,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1331,12 +1359,12 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1344,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1352,7 +1380,7 @@
         <v>41690</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1360,7 +1388,7 @@
         <v>41753</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1396,7 @@
         <v>41844</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1376,7 +1404,7 @@
         <v>41935</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1384,7 +1412,7 @@
         <v>41976</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1420,7 @@
         <v>42047</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1400,7 +1428,7 @@
         <v>42117</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1436,7 @@
         <v>42208</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1416,7 +1444,7 @@
         <v>42299</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1424,7 +1452,7 @@
         <v>42411</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1432,7 +1460,7 @@
         <v>42488</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1440,7 +1468,7 @@
         <v>42499</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1448,7 +1476,7 @@
         <v>42579</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1456,7 +1484,7 @@
         <v>42670</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1464,7 +1492,7 @@
         <v>42775</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1472,7 +1500,7 @@
         <v>42852</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1480,7 +1508,7 @@
         <v>42943</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1488,7 +1516,7 @@
         <v>43034</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1496,7 +1524,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1504,7 +1532,7 @@
         <v>43216</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1512,7 +1540,7 @@
         <v>43307</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1520,7 +1548,7 @@
         <v>43398</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1528,7 +1556,7 @@
         <v>43510</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -1536,7 +1564,7 @@
         <v>43580</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1562,12 +1590,12 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1575,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1583,7 +1611,7 @@
         <v>41689</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1591,7 +1619,7 @@
         <v>41759</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1599,7 +1627,7 @@
         <v>41768</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1635,7 @@
         <v>41850</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1615,7 +1643,7 @@
         <v>41941</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1623,7 +1651,7 @@
         <v>42060</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1631,7 +1659,7 @@
         <v>42130</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1639,7 +1667,7 @@
         <v>42214</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1647,7 +1675,7 @@
         <v>42305</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1655,7 +1683,7 @@
         <v>42424</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1663,7 +1691,7 @@
         <v>42494</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1671,7 +1699,7 @@
         <v>42585</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1679,7 +1707,7 @@
         <v>42676</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1687,7 +1715,7 @@
         <v>42789</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1695,7 +1723,7 @@
         <v>42859</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -1703,7 +1731,7 @@
         <v>42951</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -1711,7 +1739,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1719,7 +1747,7 @@
         <v>43152</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -1727,7 +1755,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1735,7 +1763,7 @@
         <v>43314</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1743,7 +1771,7 @@
         <v>43406</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1751,7 +1779,7 @@
         <v>43517</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1777,14 +1805,14 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="12.81640625" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="8.73046875" style="1"/>
+    <col min="2" max="2" width="12.796875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.73046875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1800,7 +1828,7 @@
         <v>41689</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1808,7 +1836,7 @@
         <v>41768</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1816,7 +1844,7 @@
         <v>41787</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1824,7 +1852,7 @@
         <v>41858</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1832,7 +1860,7 @@
         <v>41949</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1840,7 +1868,7 @@
         <v>42055</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1848,7 +1876,7 @@
         <v>42131</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1856,7 +1884,7 @@
         <v>42226</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1864,7 +1892,7 @@
         <v>42314</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1872,7 +1900,7 @@
         <v>42325</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
@@ -1880,7 +1908,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1888,7 +1916,7 @@
         <v>42495</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1896,7 +1924,7 @@
         <v>42591</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1904,7 +1932,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1912,7 +1940,7 @@
         <v>42781</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1920,7 +1948,7 @@
         <v>42859</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1928,7 +1956,7 @@
         <v>42949</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1936,7 +1964,7 @@
         <v>43046</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -1944,7 +1972,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1952,7 +1980,7 @@
         <v>43230</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1960,7 +1988,7 @@
         <v>43321</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1968,7 +1996,7 @@
         <v>43411</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
@@ -1976,7 +2004,7 @@
         <v>43521</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1984,7 +2012,7 @@
         <v>43536</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -2011,14 +2039,14 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.1796875" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.19921875" customWidth="1"/>
+    <col min="2" max="2" width="9.9296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2031,7 +2059,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2041,7 +2069,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2049,7 +2077,7 @@
         <v>41865</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -2057,7 +2085,7 @@
         <v>41953</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2065,7 +2093,7 @@
         <v>42080</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2073,7 +2101,7 @@
         <v>42136</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2109,7 @@
         <v>42220</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2117,7 @@
         <v>42310</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2097,7 +2125,7 @@
         <v>42425</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2105,7 +2133,7 @@
         <v>42492</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2113,7 +2141,7 @@
         <v>42590</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -2121,7 +2149,7 @@
         <v>42675</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2129,7 +2157,7 @@
         <v>42793</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2165,7 @@
         <v>42857</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -2145,7 +2173,7 @@
         <v>42954</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -2153,7 +2181,7 @@
         <v>43045</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2161,7 +2189,7 @@
         <v>43158</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2169,7 +2197,7 @@
         <v>43220</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -2177,33 +2205,33 @@
         <v>43222</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="3"/>
     </row>
   </sheetData>
@@ -2220,21 +2248,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13327362-928D-4280-A23E-95AE892B3309}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2242,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2250,7 +2278,7 @@
         <v>41691</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2258,7 +2286,7 @@
         <v>41771</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2266,7 +2294,7 @@
         <v>41858</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2274,7 +2302,7 @@
         <v>41949</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2282,7 +2310,7 @@
         <v>42061</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2290,7 +2318,7 @@
         <v>42129</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2298,7 +2326,7 @@
         <v>42215</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2306,7 +2334,7 @@
         <v>42313</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2314,7 +2342,7 @@
         <v>42425</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2322,7 +2350,7 @@
         <v>42495</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2330,7 +2358,7 @@
         <v>42585</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2338,7 +2366,7 @@
         <v>42683</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2346,7 +2374,7 @@
         <v>42788</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2354,7 +2382,7 @@
         <v>42859</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2362,7 +2390,7 @@
         <v>42950</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2370,7 +2398,7 @@
         <v>43040</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -2378,7 +2406,7 @@
         <v>43152</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2386,7 +2414,7 @@
         <v>43222</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2394,7 +2422,7 @@
         <v>43314</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2402,7 +2430,7 @@
         <v>43404</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2410,7 +2438,7 @@
         <v>43516</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -2436,9 +2464,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2456,12 +2484,12 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2469,7 +2497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2477,7 +2505,7 @@
         <v>41691</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2485,7 +2513,7 @@
         <v>41766</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2493,7 +2521,7 @@
         <v>41859</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2501,7 +2529,7 @@
         <v>41950</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2509,7 +2537,7 @@
         <v>42055</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2517,7 +2545,7 @@
         <v>42132</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2525,7 +2553,7 @@
         <v>42220</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2533,7 +2561,7 @@
         <v>42314</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2541,7 +2569,7 @@
         <v>42419</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -2549,7 +2577,7 @@
         <v>42496</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2557,7 +2585,7 @@
         <v>42587</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2565,7 +2593,7 @@
         <v>42681</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -2573,7 +2601,7 @@
         <v>42790</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -2581,7 +2609,7 @@
         <v>42863</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +2617,7 @@
         <v>42951</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2597,7 +2625,7 @@
         <v>43042</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2605,7 +2633,7 @@
         <v>43154</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -2613,7 +2641,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2621,7 +2649,7 @@
         <v>43315</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -2629,7 +2657,7 @@
         <v>43406</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2637,7 +2665,7 @@
         <v>43518</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -2664,13 +2692,13 @@
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="3"/>
-    <col min="2" max="2" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.73046875" style="3"/>
+    <col min="2" max="2" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2681,7 +2709,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2689,7 +2717,7 @@
         <v>41865</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2697,7 +2725,7 @@
         <v>41957</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2705,7 +2733,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2713,7 +2741,7 @@
         <v>42138</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2721,7 +2749,7 @@
         <v>42229</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2729,7 +2757,7 @@
         <v>42314</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -2737,7 +2765,7 @@
         <v>42429</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -2745,7 +2773,7 @@
         <v>42496</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2753,7 +2781,7 @@
         <v>42587</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2761,7 +2789,7 @@
         <v>42678</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -2769,7 +2797,7 @@
         <v>42793</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -2777,7 +2805,7 @@
         <v>42860</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -2785,7 +2813,7 @@
         <v>42951</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -2793,7 +2821,7 @@
         <v>43047</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -2801,7 +2829,7 @@
         <v>43159</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -2809,7 +2837,7 @@
         <v>43224</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -2817,7 +2845,7 @@
         <v>43320</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -2825,7 +2853,7 @@
         <v>43406</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>3</v>
       </c>
@@ -2833,7 +2861,7 @@
         <v>43523</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -2859,12 +2887,12 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2872,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2880,7 +2908,7 @@
         <v>41698</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2888,7 +2916,7 @@
         <v>41766</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2896,7 +2924,7 @@
         <v>41856</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2904,7 +2932,7 @@
         <v>41858</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2912,7 +2940,7 @@
         <v>41947</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2920,7 +2948,7 @@
         <v>42065</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2928,7 +2956,7 @@
         <v>42131</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2936,7 +2964,7 @@
         <v>42222</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2944,7 +2972,7 @@
         <v>42313</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2952,7 +2980,7 @@
         <v>42425</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2960,7 +2988,7 @@
         <v>42495</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2968,7 +2996,7 @@
         <v>42586</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2976,7 +3004,7 @@
         <v>42677</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2984,7 +3012,7 @@
         <v>42790</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2992,7 +3020,7 @@
         <v>42860</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -3000,7 +3028,7 @@
         <v>42950</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3008,7 +3036,7 @@
         <v>43041</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -3016,7 +3044,7 @@
         <v>43153</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -3024,7 +3052,7 @@
         <v>43223</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3032,7 +3060,7 @@
         <v>43314</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -3040,7 +3068,7 @@
         <v>43412</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -3048,7 +3076,7 @@
         <v>43517</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -3078,12 +3106,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3091,7 +3119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3099,7 +3127,7 @@
         <v>41697</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3107,7 +3135,7 @@
         <v>41767</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3115,7 +3143,7 @@
         <v>41858</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3123,7 +3151,7 @@
         <v>41949</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3131,7 +3159,7 @@
         <v>42061</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3139,7 +3167,7 @@
         <v>42131</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3147,7 +3175,7 @@
         <v>42222</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -3155,7 +3183,7 @@
         <v>42313</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -3163,7 +3191,7 @@
         <v>42417</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -3171,7 +3199,7 @@
         <v>42495</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -3179,7 +3207,7 @@
         <v>42586</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -3187,7 +3215,7 @@
         <v>42677</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3195,7 +3223,7 @@
         <v>42782</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -3203,7 +3231,7 @@
         <v>42859</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3211,7 +3239,7 @@
         <v>42955</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -3219,7 +3247,7 @@
         <v>43041</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -3227,7 +3255,7 @@
         <v>43146</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -3235,7 +3263,7 @@
         <v>43223</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -3243,7 +3271,7 @@
         <v>43314</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3251,7 +3279,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -3259,7 +3287,7 @@
         <v>43510</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
all sheets edited and comments added to readme page
</commit_message>
<xml_diff>
--- a/data/dates/Document_Filing_Dates.xlsx
+++ b/data/dates/Document_Filing_Dates.xlsx
@@ -8,41 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Documents\Data_Analytics\OilGasEarningsAnalysis\data\dates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E26E77A-E535-425E-90F0-5166E7901372}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589BE2DF-AACA-4E5C-B8E5-1B5AC73A0578}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="968" windowWidth="10260" windowHeight="8460" tabRatio="862" activeTab="2" xr2:uid="{3EA98B58-5733-425D-AE44-6276CE9C3BA9}"/>
+    <workbookView xWindow="368" yWindow="968" windowWidth="10260" windowHeight="8460" tabRatio="862" firstSheet="8" activeTab="14" xr2:uid="{3EA98B58-5733-425D-AE44-6276CE9C3BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="15" r:id="rId1"/>
     <sheet name="FANG" sheetId="1" r:id="rId2"/>
     <sheet name="RSPP" sheetId="2" r:id="rId3"/>
-    <sheet name="CXO see note" sheetId="3" r:id="rId4"/>
-    <sheet name="CEO see note" sheetId="4" r:id="rId5"/>
+    <sheet name="CXO" sheetId="3" r:id="rId4"/>
+    <sheet name="CEO" sheetId="4" r:id="rId5"/>
     <sheet name="MDU" sheetId="5" r:id="rId6"/>
     <sheet name="PE" sheetId="6" r:id="rId7"/>
     <sheet name="MRO" sheetId="7" r:id="rId8"/>
     <sheet name="LPI" sheetId="8" r:id="rId9"/>
-    <sheet name="NFX see note" sheetId="9" r:id="rId10"/>
-    <sheet name="ECA see note" sheetId="13" r:id="rId11"/>
+    <sheet name="NFX" sheetId="9" r:id="rId10"/>
+    <sheet name="ECA" sheetId="13" r:id="rId11"/>
     <sheet name="GPOR" sheetId="10" r:id="rId12"/>
     <sheet name="RRC" sheetId="11" r:id="rId13"/>
     <sheet name="EQT" sheetId="12" r:id="rId14"/>
-    <sheet name="SM (added for me if possible)" sheetId="14" r:id="rId15"/>
+    <sheet name="SM" sheetId="14" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'CXO see note'!$A$3:$B$46</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'ECA see note'!$A$3:$B$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CXO!$A$3:$B$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">ECA!$A$1:$B$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">EQT!$A$1:$B$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">FANG!$A$1:$B$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">GPOR!$A$1:$B$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">LPI!$A$1:$B$46</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MDU!$A$1:$B$45</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">MRO!$A$1:$B$48</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'NFX see note'!$A$3:$B$23</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">NFX!$A$1:$B$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PE!$A$1:$B$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">RRC!$A$1:$B$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RSPP!$A$1:$B$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">'SM (added for me if possible)'!$A$1:$B$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">SM!$A$1:$B$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="20">
   <si>
     <t>Filings</t>
   </si>
@@ -84,12 +84,6 @@
   </si>
   <si>
     <t>*Has no 10Ks because they're a foreign company I think. We might want to replace this one</t>
-  </si>
-  <si>
-    <t>**they started mid 2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>**Newfield was bought by Encana at the end of 2018. They merged but you wouldn't see that until you see the 8Ks or the 425s</t>
@@ -120,6 +114,12 @@
   </si>
   <si>
     <t xml:space="preserve">3. close at day before filing date to close 3 months (before next filing)? </t>
+  </si>
+  <si>
+    <t>PE they started mid 2014</t>
+  </si>
+  <si>
+    <t>(NFX)Newfield was bought by Encana at the end of 2018. They merged but you wouldn't see that until you see the 8Ks or the 425s</t>
   </si>
 </sst>
 </file>
@@ -518,52 +518,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4347CB-D72A-415A-B9FD-4EDC7C72C60F}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="O6" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="O7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="O8" s="4" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -573,10 +596,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63EF6CC7-26D8-4A7A-A502-BD1E255BE555}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -584,124 +607,132 @@
     <col min="2" max="2" width="10.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>41698</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>41759</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>41698</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>41850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>41759</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>41941</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3">
-        <v>41850</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42059</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3">
-        <v>41941</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>42059</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
-        <v>42130</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>42221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42424</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <v>42312</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42493</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3">
-        <v>42424</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42585</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="3">
-        <v>42493</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42675</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3">
-        <v>42585</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42787</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="3">
-        <v>42675</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42857</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="3">
-        <v>42787</v>
+        <v>42948</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -709,15 +740,15 @@
         <v>4</v>
       </c>
       <c r="B17" s="3">
-        <v>42857</v>
+        <v>43039</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3">
-        <v>42948</v>
+        <v>43151</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
@@ -725,15 +756,15 @@
         <v>4</v>
       </c>
       <c r="B19" s="3">
-        <v>43039</v>
+        <v>43221</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20" s="3">
-        <v>43151</v>
+        <v>43312</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
@@ -741,33 +772,17 @@
         <v>4</v>
       </c>
       <c r="B21" s="3">
-        <v>43221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3">
-        <v>43312</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="3">
         <v>43404</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:B23" xr:uid="{AAC71BF4-6E59-4E44-BFF8-03072FDF897B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B23">
-      <sortCondition ref="B3:B23"/>
+  <autoFilter ref="A1:B21" xr:uid="{AAC71BF4-6E59-4E44-BFF8-03072FDF897B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B21">
+      <sortCondition ref="B1:B21"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B42">
-    <sortCondition ref="A3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B40">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -775,10 +790,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{532AA2A0-7A1E-46EF-A252-90C77DFE0331}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -786,111 +801,107 @@
     <col min="2" max="2" width="9.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42793</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>42859</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>42793</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>42941</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>42859</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>43048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="3">
-        <v>42941</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>43157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3">
-        <v>43048</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>43223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>43157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>43314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3">
-        <v>43223</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>43410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3">
-        <v>43314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>43524</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <v>43410</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3">
-        <v>43524</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
         <v>43587</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
@@ -905,16 +916,10 @@
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B22" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:B22" xr:uid="{A6387B7E-A334-48B7-B40A-0563183242DD}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:B22">
-      <sortCondition ref="B3:B22"/>
+  <autoFilter ref="A1:B20" xr:uid="{A6387B7E-A334-48B7-B40A-0563183242DD}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
+      <sortCondition ref="B1:B20"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1586,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539C74E3-D5C1-4CB1-BADB-DA612265659D}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2035,7 +2040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9686624-2BCC-4283-AC4D-D0F6B59205DE}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -2243,22 +2248,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13327362-928D-4280-A23E-95AE892B3309}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A3:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
@@ -2477,7 +2475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94A8DCB2-D7BE-4A47-9585-4F562C82DBBA}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2683,10 +2681,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27EBFEEE-31A4-4E38-A9F6-5FA1B2E0DF74}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2695,18 +2693,15 @@
     <col min="2" max="2" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2714,7 +2709,7 @@
         <v>41865</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -2722,7 +2717,7 @@
         <v>41957</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2730,7 +2725,7 @@
         <v>42074</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2738,7 +2733,7 @@
         <v>42138</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2746,7 +2741,7 @@
         <v>42229</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -2754,7 +2749,7 @@
         <v>42314</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -2762,7 +2757,7 @@
         <v>42429</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -2770,7 +2765,7 @@
         <v>42496</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -2778,7 +2773,7 @@
         <v>42587</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -2786,7 +2781,7 @@
         <v>42678</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -2794,7 +2789,7 @@
         <v>42793</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -2802,7 +2797,7 @@
         <v>42860</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -2810,7 +2805,7 @@
         <v>42951</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -2818,7 +2813,7 @@
         <v>43047</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -2880,7 +2875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA5AFAA-7824-4617-819B-4E92B4149268}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -3099,7 +3094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5F963A-41EF-4CFB-B617-A23EE18B99D9}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>